<commit_message>
skyopc metadata update after 2022 instrument relocation
</commit_message>
<xml_diff>
--- a/metadata/skyopc_metadata.xlsx
+++ b/metadata/skyopc_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7465AA75-5428-8B49-BF12-DE9EBFBB97DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AD98B5-A133-174E-8804-8311A6C80170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-3140" windowWidth="28020" windowHeight="19040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6080" yWindow="500" windowWidth="32320" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global-attributes" sheetId="1" r:id="rId1"/>
@@ -223,9 +223,6 @@
     <t>Summit, Greenland, Greenland Ice Sheet</t>
   </si>
   <si>
-    <t>Data collection start: 2019-06-01T00:00:00</t>
-  </si>
-  <si>
     <t>3267 m</t>
   </si>
   <si>
@@ -235,14 +232,20 @@
     <t>Point measurements of aerosol size distribution at Summit Station, Greenland</t>
   </si>
   <si>
-    <t>72.578590N -38.452693E</t>
-  </si>
-  <si>
-    <t>Data are corrected for particle loss in the inlet</t>
+    <t>timeSeries</t>
+  </si>
+  <si>
+    <t>72.573730N -38.470528E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data collection start: 2019-06-01T00:00:00. Note that after 21st August 2022, the SKYOPC was moved from the MSF building to the AWO building (within the clean air sector at Summit) and now shares a TSP Pm10 inlet (part#TSPL-1) with the NOAA GML aerosol instrumentation. Qc'ing for local station pollution accounts for this change of location. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data are corrected for particle loss in the custom inlet prior to 21st August 2022. After this date the inlet was replaced with a TSP Pm10 inlet (part#TSPL-1) and no inlet loss correction has been applied. </t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Acknowledgement of the following grants is required: NSFGE Grant Award number: </t>
+      <t xml:space="preserve">Acknowledgement of the following grants is required: NSFGEO Grant Award number: </t>
     </r>
     <r>
       <rPr>
@@ -260,11 +263,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>NERC Grant Award number NE/S00906X/1</t>
+      <t>NERC Grant Award numbers NE/S00906X/1 and NE/X002403/1</t>
     </r>
-  </si>
-  <si>
-    <t>timeSeries</t>
   </si>
 </sst>
 </file>
@@ -382,11 +382,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -410,7 +410,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -704,10 +704,10 @@
   <dimension ref="A1:M1003"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="245" zoomScaleNormal="245" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -819,7 +819,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -937,7 +937,7 @@
         <v>31</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -969,7 +969,7 @@
         <v>37</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -977,7 +977,7 @@
         <v>38</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1016,7 +1016,7 @@
         <v>42</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1040,7 +1040,7 @@
         <v>46</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -1048,7 +1048,7 @@
         <v>47</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>